<commit_message>
Updated codes specifically for Manuscript III analysis
Customized code to analyze the data
</commit_message>
<xml_diff>
--- a/result_acidosis.xlsx
+++ b/result_acidosis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\GitHub\ChangValiante2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\ChangValiante2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25DFD42-E7F6-4D74-B30D-1D23ECFFC1E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A9974B-F1BC-48B1-8265-6BC04C593CFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24585" yWindow="5970" windowWidth="22485" windowHeight="10485" activeTab="9" xr2:uid="{B8EBFF42-C88B-4EC5-B765-97FE0960549A}"/>
+    <workbookView xWindow="-42310" yWindow="340" windowWidth="18851" windowHeight="11023" firstSheet="4" activeTab="9" xr2:uid="{B8EBFF42-C88B-4EC5-B765-97FE0960549A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="34">
   <si>
     <t>Treatment Group</t>
   </si>
@@ -127,6 +127,21 @@
   </si>
   <si>
     <t>pH 6.9 (round 2)</t>
+  </si>
+  <si>
+    <t>Duration (s), median</t>
+  </si>
+  <si>
+    <t>Duration (s), IQR</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>KS D stat</t>
+  </si>
+  <si>
+    <t>Cliffs D</t>
   </si>
 </sst>
 </file>
@@ -482,7 +497,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -492,21 +507,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B19DD4-5EC5-437F-A176-2D4FB8CEABFE}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E6" activeCellId="1" sqref="B6 E6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -530,24 +545,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>24.295097142857134</v>
+        <v>24.681840000000136</v>
       </c>
       <c r="C2">
-        <v>4.2055420466635587</v>
+        <v>5.4134399999998237</v>
       </c>
       <c r="D2">
-        <v>0.22438573607749462</v>
+        <v>0.2243857360774992</v>
       </c>
       <c r="E2">
-        <v>370835.33563467354</v>
+        <v>391781.4454027852</v>
       </c>
       <c r="F2">
-        <v>174367.00074806955</v>
+        <v>346234.2190919249</v>
       </c>
       <c r="G2">
         <v>1.8483653486959732E-2</v>
@@ -559,24 +574,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>27.017431272727414</v>
+        <v>26.859647999999652</v>
       </c>
       <c r="C3">
-        <v>3.0864193931922252</v>
+        <v>2.9741279999996095</v>
       </c>
       <c r="D3">
         <v>5.5616357874621707E-2</v>
       </c>
       <c r="E3">
-        <v>416357.69890750916</v>
+        <v>426501.76747243921</v>
       </c>
       <c r="F3">
-        <v>89181.335831481498</v>
+        <v>128338.2572215955</v>
       </c>
       <c r="G3">
         <v>0.58262490575757342</v>
@@ -588,24 +603,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>25.63560436363613</v>
+        <v>24.66172799999913</v>
       </c>
       <c r="C4">
-        <v>3.6129870322754831</v>
+        <v>5.5079279999995379</v>
       </c>
       <c r="D4">
-        <v>0.36060068892327868</v>
+        <v>0.3606006889232749</v>
       </c>
       <c r="E4">
-        <v>297103.81587336335</v>
+        <v>304965.69681405724</v>
       </c>
       <c r="F4">
-        <v>39224.61150669062</v>
+        <v>73571.530899229925</v>
       </c>
       <c r="G4">
         <v>0.26298432321270676</v>
@@ -617,23 +632,55 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <v>9.7845465865037638E-3</v>
       </c>
+      <c r="C6">
+        <v>0.40367965367965369</v>
+      </c>
+      <c r="D6">
+        <v>-0.44805194805194803</v>
+      </c>
       <c r="E6">
         <v>2.7373436999226213E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0.36255411255411252</v>
+      </c>
+      <c r="G6">
+        <v>-8.4415584415584416E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -653,7 +700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -667,43 +714,43 @@
         <v>56.211469393962304</v>
       </c>
       <c r="E10">
-        <v>4.2486206353265743</v>
+        <v>4.2486206353265734</v>
       </c>
       <c r="F10">
         <v>1.8193583638088581E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>912.90602788433409</v>
+        <v>912.90602788433432</v>
       </c>
       <c r="C11">
         <v>69</v>
       </c>
       <c r="D11">
-        <v>13.230522143251219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13.230522143251221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12">
-        <v>1025.3289666722587</v>
+        <v>1025.328966672259</v>
       </c>
       <c r="C12">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -714,7 +761,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -728,13 +775,13 @@
         <v>-2.7223341298702799</v>
       </c>
       <c r="E16">
-        <v>-0.48371866220922222</v>
+        <v>-0.48371866220922177</v>
       </c>
       <c r="F16">
-        <v>1.3212819206172899E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.321281920617301E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -748,13 +795,13 @@
         <v>-1.3405072207789921</v>
       </c>
       <c r="E17">
-        <v>1.7598198582378894</v>
+        <v>1.7598198582378903</v>
       </c>
       <c r="F17">
-        <v>0.55708216341391781</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.55708216341391792</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -762,7 +809,7 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>-1.6515305656663486</v>
+        <v>-1.651530565666349</v>
       </c>
       <c r="D18">
         <v>1.3818269090912878</v>
@@ -771,15 +818,15 @@
         <v>4.4151843838489242</v>
       </c>
       <c r="F18">
-        <v>0.52274509095321808</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.52274509095321819</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -799,7 +846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -819,7 +866,7 @@
         <v>2.6123844409619467E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -833,7 +880,7 @@
         <v>15808632148.799921</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -844,12 +891,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -860,7 +907,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -880,7 +927,7 @@
         <v>0.34184591624259864</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -900,7 +947,7 @@
         <v>0.23272995686606468</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -933,12 +980,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -970,7 +1017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -999,7 +1046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1028,7 +1075,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1057,7 +1104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1068,12 +1115,12 @@
         <v>2.7773148291571074E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1093,7 +1140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1160,7 @@
         <v>1.1216401633771319E-15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1127,7 +1174,7 @@
         <v>31.749020380082129</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1138,12 +1185,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1154,7 +1201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1174,7 +1221,7 @@
         <v>9.5987473525127598E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1194,7 +1241,7 @@
         <v>3.6000287580939538E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1214,12 +1261,12 @@
         <v>1.135991416489901E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1239,7 +1286,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1259,7 +1306,7 @@
         <v>4.7467163819920818E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1273,7 +1320,7 @@
         <v>2111183482.1113365</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1284,12 +1331,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1300,7 +1347,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1320,7 +1367,7 @@
         <v>0.19232133959083142</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1340,7 +1387,7 @@
         <v>3.0223341130342085E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1373,13 +1420,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1458,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1440,7 +1487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1469,7 +1516,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1498,7 +1545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1509,12 +1556,12 @@
         <v>9.8364125695967995E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +1581,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1554,7 +1601,7 @@
         <v>8.6418320225013973E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1568,7 +1615,7 @@
         <v>5578.5624302162141</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1579,12 +1626,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1595,7 +1642,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1615,7 +1662,7 @@
         <v>9.047317915102937E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1635,7 +1682,7 @@
         <v>0.48400509532280178</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1655,12 +1702,12 @@
         <v>1.9760865566389452E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1680,7 +1727,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1700,7 +1747,7 @@
         <v>8.0377542121105136E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1714,7 +1761,7 @@
         <v>76208947358.237259</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1725,12 +1772,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -1741,7 +1788,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1761,7 +1808,7 @@
         <v>9.3525771843296912E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1781,7 +1828,7 @@
         <v>0.17772216298692123</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1814,13 +1861,13 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1852,7 +1899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1881,7 +1928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1910,7 +1957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1939,7 +1986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1950,12 +1997,12 @@
         <v>3.0035332405743277E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1975,7 +2022,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1995,7 +2042,7 @@
         <v>8.5830811916006691E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2009,7 +2056,7 @@
         <v>53.096400124597857</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2020,12 +2067,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2036,7 +2083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2056,7 +2103,7 @@
         <v>9.2053211554544379E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2076,7 +2123,7 @@
         <v>1.3514581863284247E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2096,12 +2143,12 @@
         <v>4.91058377627418E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2121,7 +2168,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2141,7 +2188,7 @@
         <v>1.7737277870311691E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2155,7 +2202,7 @@
         <v>30.964468442292173</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2166,12 +2213,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2182,7 +2229,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2202,7 +2249,7 @@
         <v>2.8816316959266008E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2222,7 +2269,7 @@
         <v>1.2176546111917208E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2255,12 +2302,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2292,7 +2339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2321,7 +2368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2350,7 +2397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2379,7 +2426,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2390,12 +2437,12 @@
         <v>3.8091018846294254E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2415,7 +2462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2435,7 +2482,7 @@
         <v>1.3060384118764952E-8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2449,7 +2496,7 @@
         <v>57.472360148078579</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2460,12 +2507,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2476,7 +2523,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2496,7 +2543,7 @@
         <v>6.712528310970356E-8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2516,7 +2563,7 @@
         <v>8.699872122181207E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2536,12 +2583,12 @@
         <v>1.2336754100505942E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2561,7 +2608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2581,7 +2628,7 @@
         <v>5.8465516133926445E-13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2595,7 +2642,7 @@
         <v>1326275100.5041475</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2606,12 +2653,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2622,7 +2669,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2642,7 +2689,7 @@
         <v>3.294946870902038E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2662,7 +2709,7 @@
         <v>0.62273697327317445</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2695,12 +2742,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2732,7 +2779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2761,7 +2808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2790,12 +2837,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2819,12 +2866,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2856,7 +2903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2885,7 +2932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2914,7 +2961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2943,7 +2990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2954,12 +3001,12 @@
         <v>0.14003469339668584</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2979,7 +3026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2999,7 +3046,7 @@
         <v>0.16598164038683369</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3013,7 +3060,7 @@
         <v>25.971569021456617</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3024,12 +3071,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3040,7 +3087,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3060,7 +3107,7 @@
         <v>0.22837331586627374</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3080,7 +3127,7 @@
         <v>0.22002278150766386</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3100,12 +3147,12 @@
         <v>0.92967906107179099</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3125,7 +3172,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3145,7 +3192,7 @@
         <v>3.6700599253392687E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -3159,7 +3206,7 @@
         <v>1837079449.1406765</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -3170,12 +3217,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3186,7 +3233,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3206,7 +3253,7 @@
         <v>0.18097790087497956</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3226,7 +3273,7 @@
         <v>3.1139678851932473E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -3259,13 +3306,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3297,7 +3344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3326,7 +3373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -3355,7 +3402,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -3384,7 +3431,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3395,12 +3442,12 @@
         <v>8.7276419421678536E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3420,7 +3467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3440,7 +3487,7 @@
         <v>9.6745213828038746E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3454,7 +3501,7 @@
         <v>63.830726567831306</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3465,12 +3512,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3481,7 +3528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3501,7 +3548,7 @@
         <v>5.639277554925215E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3521,7 +3568,7 @@
         <v>1.9236885913630153E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3541,12 +3588,12 @@
         <v>3.2750145306927325E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3566,7 +3613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3586,7 +3633,7 @@
         <v>1.3122524387752867E-9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -3600,7 +3647,7 @@
         <v>13255828792.769474</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -3611,12 +3658,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -3627,7 +3674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3647,7 +3694,7 @@
         <v>5.2319694249711723E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3667,7 +3714,7 @@
         <v>1.4954505947883945E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -3700,9 +3747,9 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3734,7 +3781,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -3763,7 +3810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3792,7 +3839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -3821,7 +3868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3832,12 +3879,12 @@
         <v>1.3741431386418531E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3857,7 +3904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3877,7 +3924,7 @@
         <v>1.9737387769715659E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3891,7 +3938,7 @@
         <v>62.559236836641091</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -3902,12 +3949,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3918,7 +3965,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3938,7 +3985,7 @@
         <v>1.2397734061586618E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -3958,7 +4005,7 @@
         <v>1.7891919382010735E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3978,12 +4025,12 @@
         <v>1.2126746409293232E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -4003,7 +4050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -4023,7 +4070,7 @@
         <v>5.9373596511898177E-8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -4037,7 +4084,7 @@
         <v>14222853551.811354</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -4048,12 +4095,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -4064,7 +4111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -4084,7 +4131,7 @@
         <v>6.8629928745286728E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -4104,7 +4151,7 @@
         <v>2.4428744416593595E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Stage 3 Analysis Complete
I've updated stage 2 to include stage 3 analysis.
I've turned the frequency content analysis script into a function.
I've written updates for the scripts in onenote
</commit_message>
<xml_diff>
--- a/result_acidosis.xlsx
+++ b/result_acidosis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\ChangValiante2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A9974B-F1BC-48B1-8265-6BC04C593CFE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B85904-37DD-400F-8111-EB0918B9B240}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42310" yWindow="340" windowWidth="18851" windowHeight="11023" firstSheet="4" activeTab="9" xr2:uid="{B8EBFF42-C88B-4EC5-B765-97FE0960549A}"/>
+    <workbookView xWindow="2657" yWindow="2657" windowWidth="18851" windowHeight="11023" firstSheet="4" activeTab="9" xr2:uid="{B8EBFF42-C88B-4EC5-B765-97FE0960549A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="41">
   <si>
     <t>Treatment Group</t>
   </si>
@@ -142,6 +142,27 @@
   </si>
   <si>
     <t>Cliffs D</t>
+  </si>
+  <si>
+    <t>Intensity (mV^2/s), median</t>
+  </si>
+  <si>
+    <t>Intensity (mV^2/s), IQR</t>
+  </si>
+  <si>
+    <t>Dominant Frequency, median</t>
+  </si>
+  <si>
+    <t>Dominant Frequency, IQR</t>
+  </si>
+  <si>
+    <t>PostTest</t>
+  </si>
+  <si>
+    <t>one-way ANOVA, dominant frequency</t>
+  </si>
+  <si>
+    <t>Multiple Comparison (Tukey-Kramer method), dominant frequency</t>
   </si>
 </sst>
 </file>
@@ -505,15 +526,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B19DD4-5EC5-437F-A176-2D4FB8CEABFE}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:F30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,10 +548,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -539,13 +560,19 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -559,22 +586,31 @@
         <v>0.2243857360774992</v>
       </c>
       <c r="E2">
-        <v>391781.4454027852</v>
+        <v>378566.68421590159</v>
       </c>
       <c r="F2">
-        <v>346234.2190919249</v>
+        <v>346753.61093470646</v>
       </c>
       <c r="G2">
-        <v>1.8483653486959732E-2</v>
+        <v>1.6455119890529613E-2</v>
       </c>
       <c r="H2">
         <v>1.462327267180874E-3</v>
       </c>
+      <c r="I2">
+        <v>15.418228149414063</v>
+      </c>
       <c r="J2">
+        <v>16.054031372070313</v>
+      </c>
+      <c r="K2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L2">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -588,24 +624,33 @@
         <v>5.5616357874621707E-2</v>
       </c>
       <c r="E3">
-        <v>426501.76747243921</v>
+        <v>414085.71964627929</v>
       </c>
       <c r="F3">
-        <v>128338.2572215955</v>
+        <v>125928.82214807905</v>
       </c>
       <c r="G3">
-        <v>0.58262490575757342</v>
+        <v>0.57979270012249917</v>
       </c>
       <c r="H3">
         <v>5.6066262743570405E-14</v>
       </c>
+      <c r="I3">
+        <v>16.212982177734375</v>
+      </c>
       <c r="J3">
+        <v>7.8680648803710938</v>
+      </c>
+      <c r="K3">
+        <v>6.5940482305243589E-2</v>
+      </c>
+      <c r="L3">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>24.66172799999913</v>
@@ -617,22 +662,31 @@
         <v>0.3606006889232749</v>
       </c>
       <c r="E4">
-        <v>304965.69681405724</v>
+        <v>295410.50212958449</v>
       </c>
       <c r="F4">
-        <v>73571.530899229925</v>
+        <v>72611.518940786162</v>
       </c>
       <c r="G4">
-        <v>0.26298432321270676</v>
+        <v>0.38094222869523064</v>
       </c>
       <c r="H4">
         <v>1.3946154254762533E-6</v>
       </c>
+      <c r="I4">
+        <v>18.120391845703125</v>
+      </c>
       <c r="J4">
+        <v>6.1196060180664063</v>
+      </c>
+      <c r="K4">
+        <v>0.97235305289678287</v>
+      </c>
+      <c r="L4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -651,8 +705,17 @@
       <c r="G5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -672,15 +735,24 @@
         <v>0.36255411255411252</v>
       </c>
       <c r="G6">
-        <v>-8.4415584415584416E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>-8.2251082251082255E-2</v>
+      </c>
+      <c r="I6">
+        <v>6.8571263419851772E-2</v>
+      </c>
+      <c r="J6">
+        <v>0.3214285714285714</v>
+      </c>
+      <c r="K6">
+        <v>0.21536796536796537</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -700,7 +772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -720,7 +792,7 @@
         <v>1.8193583638088581E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -734,7 +806,7 @@
         <v>13.230522143251221</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -745,12 +817,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -761,7 +833,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -851,19 +923,19 @@
         <v>17</v>
       </c>
       <c r="B22">
-        <v>121549778084.45186</v>
+        <v>120001217405.62329</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
       <c r="D22">
-        <v>60774889042.225929</v>
+        <v>60000608702.811646</v>
       </c>
       <c r="E22">
-        <v>3.8444116145013552</v>
+        <v>3.8279595183402142</v>
       </c>
       <c r="F22">
-        <v>2.6123844409619467E-2</v>
+        <v>2.6513505941062845E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,13 +943,13 @@
         <v>18</v>
       </c>
       <c r="B23">
-        <v>1090795618267.1946</v>
+        <v>1081527111417.6011</v>
       </c>
       <c r="C23">
         <v>69</v>
       </c>
       <c r="D23">
-        <v>15808632148.799921</v>
+        <v>15674305962.573929</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -885,7 +957,7 @@
         <v>19</v>
       </c>
       <c r="B24">
-        <v>1212345396351.6465</v>
+        <v>1201528328823.2244</v>
       </c>
       <c r="C24">
         <v>71</v>
@@ -915,16 +987,16 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>-122904.04343536115</v>
+        <v>-124268.14471554037</v>
       </c>
       <c r="D28">
-        <v>-45522.363272835792</v>
+        <v>-47215.922551188734</v>
       </c>
       <c r="E28">
-        <v>31859.316889689566</v>
+        <v>29836.299613162904</v>
       </c>
       <c r="F28">
-        <v>0.34184591624259864</v>
+        <v>0.31262597079141563</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -935,16 +1007,16 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>-33436.737535849097</v>
+        <v>-36062.88023059594</v>
       </c>
       <c r="D29">
-        <v>73731.519761310192</v>
+        <v>70649.100601090759</v>
       </c>
       <c r="E29">
-        <v>180899.77705846948</v>
+        <v>177361.08143277746</v>
       </c>
       <c r="F29">
-        <v>0.23272995686606468</v>
+        <v>0.25857075570236077</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -955,16 +1027,162 @@
         <v>3</v>
       </c>
       <c r="C30">
-        <v>14400.547871789167</v>
+        <v>13458.108510023478</v>
       </c>
       <c r="D30">
-        <v>119253.88303414598</v>
+        <v>117865.02315227949</v>
       </c>
       <c r="E30">
-        <v>224107.2181965028</v>
+        <v>222271.93779453551</v>
       </c>
       <c r="F30">
-        <v>2.1957309826135751E-2</v>
+        <v>2.3150607221503416E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34">
+        <v>181.91019926456897</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>90.955099632284487</v>
+      </c>
+      <c r="E34">
+        <v>2.3778586898253011</v>
+      </c>
+      <c r="F34">
+        <v>0.10030954804940632</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>2639.3081731398906</v>
+      </c>
+      <c r="C35">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>38.25084308898392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36">
+        <v>2821.2183724044598</v>
+      </c>
+      <c r="C36">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>-0.41542396957261962</v>
+      </c>
+      <c r="D40">
+        <v>3.3909505208333357</v>
+      </c>
+      <c r="E40">
+        <v>7.1973250112392915</v>
+      </c>
+      <c r="F40">
+        <v>9.0451079898563491E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>-2.5260506183858746</v>
+      </c>
+      <c r="D41">
+        <v>2.7455139160156286</v>
+      </c>
+      <c r="E41">
+        <v>8.0170784504171309</v>
+      </c>
+      <c r="F41">
+        <v>0.42963217002346643</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>-5.8031310275508989</v>
+      </c>
+      <c r="D42">
+        <v>-0.64543660481770715</v>
+      </c>
+      <c r="E42">
+        <v>4.5122578179154846</v>
+      </c>
+      <c r="F42">
+        <v>0.95171280623759369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>